<commit_message>
fixed the excel headers for maintenance report
</commit_message>
<xml_diff>
--- a/superadmin/excel-reports/maintenance.xlsx
+++ b/superadmin/excel-reports/maintenance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Civic-ITAM\superadmin\excel-reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6183EEE5-4EA5-4D1D-A716-6D99D3B05701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550695C3-F2AB-44F7-BA8F-2F08563DA783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="21948" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Leave Application List" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Leave Application List'!$2:$2</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Leave Application List'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="150001"/>
   <extLst>
@@ -30,13 +30,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Remarks</t>
-  </si>
-  <si>
     <t>Request ID</t>
-  </si>
-  <si>
-    <t>Maintenance Name</t>
   </si>
   <si>
     <t>Category</t>
@@ -49,6 +43,12 @@
   </si>
   <si>
     <t>MAINTENANCE REPORTS</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Remarks</t>
   </si>
 </sst>
 </file>
@@ -177,10 +177,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -463,249 +462,416 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G66"/>
+  <dimension ref="A1:F122"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="19.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.77734375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="28" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="25" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="63" customHeight="1">
-      <c r="B1" s="11" t="s">
-        <v>6</v>
+    <row r="1" spans="1:6" ht="54" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>4</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-    </row>
-    <row r="2" spans="2:7" s="2" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
-      <c r="B2" s="3" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" ht="19.5" customHeight="1" thickBot="1">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="19.5" customHeight="1" thickTop="1">
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="2:7" ht="19.5" customHeight="1">
-      <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="2:7" ht="19.5" customHeight="1">
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="2:7" ht="19.5" customHeight="1">
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="2:7" ht="19.5" customHeight="1">
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="2:7" ht="19.5" customHeight="1">
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="2:7" ht="19.5" customHeight="1">
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="2:7" ht="19.5" customHeight="1">
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="2:7" ht="19.5" customHeight="1">
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="2:7" ht="19.5" customHeight="1">
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="2:7" ht="19.5" customHeight="1">
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="2:7" ht="19.5" customHeight="1">
-      <c r="F14" s="12"/>
-    </row>
-    <row r="15" spans="2:7" ht="19.5" customHeight="1">
-      <c r="F15" s="12"/>
-    </row>
-    <row r="16" spans="2:7" ht="19.5" customHeight="1">
-      <c r="F16" s="12"/>
-    </row>
-    <row r="17" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F18" s="12"/>
-    </row>
-    <row r="19" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F22" s="12"/>
-    </row>
-    <row r="23" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F23" s="12"/>
-    </row>
-    <row r="24" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F24" s="12"/>
-    </row>
-    <row r="25" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F25" s="12"/>
-    </row>
-    <row r="26" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F26" s="12"/>
-    </row>
-    <row r="27" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F27" s="12"/>
-    </row>
-    <row r="28" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F28" s="12"/>
-    </row>
-    <row r="29" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F29" s="12"/>
-    </row>
-    <row r="30" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F30" s="12"/>
-    </row>
-    <row r="31" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F31" s="12"/>
-    </row>
-    <row r="32" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F32" s="12"/>
-    </row>
-    <row r="33" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F33" s="12"/>
-    </row>
-    <row r="34" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F34" s="12"/>
-    </row>
-    <row r="35" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F35" s="12"/>
-    </row>
-    <row r="36" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F36" s="12"/>
-    </row>
-    <row r="37" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F37" s="12"/>
-    </row>
-    <row r="38" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F38" s="12"/>
-    </row>
-    <row r="39" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F39" s="12"/>
-    </row>
-    <row r="40" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F40" s="12"/>
-    </row>
-    <row r="41" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F41" s="12"/>
-    </row>
-    <row r="42" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F42" s="12"/>
-    </row>
-    <row r="43" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F43" s="12"/>
-    </row>
-    <row r="44" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F44" s="12"/>
-    </row>
-    <row r="45" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F45" s="12"/>
-    </row>
-    <row r="46" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F46" s="12"/>
-    </row>
-    <row r="47" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F47" s="12"/>
-    </row>
-    <row r="48" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F48" s="12"/>
-    </row>
-    <row r="49" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F49" s="12"/>
-    </row>
-    <row r="50" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F50" s="12"/>
-    </row>
-    <row r="51" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F51" s="12"/>
-    </row>
-    <row r="52" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F52" s="12"/>
-    </row>
-    <row r="53" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F53" s="12"/>
-    </row>
-    <row r="54" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F54" s="12"/>
-    </row>
-    <row r="55" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F55" s="12"/>
-    </row>
-    <row r="56" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F56" s="12"/>
-    </row>
-    <row r="57" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F57" s="12"/>
-    </row>
-    <row r="58" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F58" s="12"/>
-    </row>
-    <row r="59" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F59" s="12"/>
-    </row>
-    <row r="60" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F60" s="12"/>
-    </row>
-    <row r="61" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F61" s="12"/>
-    </row>
-    <row r="62" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F62" s="12"/>
-    </row>
-    <row r="63" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F63" s="12"/>
-    </row>
-    <row r="64" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F64" s="12"/>
-    </row>
-    <row r="65" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F65" s="12"/>
-    </row>
-    <row r="66" spans="6:6" ht="19.5" customHeight="1">
-      <c r="F66" s="12"/>
+    </row>
+    <row r="3" spans="1:6" ht="19.5" customHeight="1" thickTop="1">
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" ht="19.5" customHeight="1">
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:6" ht="19.5" customHeight="1">
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" ht="19.5" customHeight="1">
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" ht="19.5" customHeight="1">
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" ht="19.5" customHeight="1">
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" ht="19.5" customHeight="1">
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" ht="19.5" customHeight="1">
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:6" ht="19.5" customHeight="1">
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="1:6" ht="19.5" customHeight="1">
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="1:6" ht="19.5" customHeight="1">
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="1:6" ht="19.5" customHeight="1">
+      <c r="E14" s="11"/>
+    </row>
+    <row r="15" spans="1:6" ht="19.5" customHeight="1">
+      <c r="E15" s="11"/>
+    </row>
+    <row r="16" spans="1:6" ht="19.5" customHeight="1">
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E17" s="11"/>
+    </row>
+    <row r="18" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E18" s="11"/>
+    </row>
+    <row r="19" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E20" s="11"/>
+    </row>
+    <row r="21" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E22" s="11"/>
+    </row>
+    <row r="23" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E23" s="11"/>
+    </row>
+    <row r="24" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E24" s="11"/>
+    </row>
+    <row r="25" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E26" s="11"/>
+    </row>
+    <row r="27" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E27" s="11"/>
+    </row>
+    <row r="28" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E28" s="11"/>
+    </row>
+    <row r="29" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E29" s="11"/>
+    </row>
+    <row r="30" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E30" s="11"/>
+    </row>
+    <row r="31" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E31" s="11"/>
+    </row>
+    <row r="32" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E32" s="11"/>
+    </row>
+    <row r="33" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E33" s="11"/>
+    </row>
+    <row r="34" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E34" s="11"/>
+    </row>
+    <row r="35" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E35" s="11"/>
+    </row>
+    <row r="36" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E36" s="11"/>
+    </row>
+    <row r="37" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E37" s="11"/>
+    </row>
+    <row r="38" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E38" s="11"/>
+    </row>
+    <row r="39" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E39" s="11"/>
+    </row>
+    <row r="40" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E40" s="11"/>
+    </row>
+    <row r="41" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E41" s="11"/>
+    </row>
+    <row r="42" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E42" s="11"/>
+    </row>
+    <row r="43" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E43" s="11"/>
+    </row>
+    <row r="44" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E44" s="11"/>
+    </row>
+    <row r="45" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E45" s="11"/>
+    </row>
+    <row r="46" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E46" s="11"/>
+    </row>
+    <row r="47" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E47" s="11"/>
+    </row>
+    <row r="48" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E48" s="11"/>
+    </row>
+    <row r="49" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E49" s="11"/>
+    </row>
+    <row r="50" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E50" s="11"/>
+    </row>
+    <row r="51" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E51" s="11"/>
+    </row>
+    <row r="52" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E52" s="11"/>
+    </row>
+    <row r="53" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E53" s="11"/>
+    </row>
+    <row r="54" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E54" s="11"/>
+    </row>
+    <row r="55" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E55" s="11"/>
+    </row>
+    <row r="56" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E56" s="11"/>
+    </row>
+    <row r="57" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E57" s="11"/>
+    </row>
+    <row r="58" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E58" s="11"/>
+    </row>
+    <row r="59" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E59" s="11"/>
+    </row>
+    <row r="60" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E60" s="11"/>
+    </row>
+    <row r="61" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E61" s="11"/>
+    </row>
+    <row r="62" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E62" s="11"/>
+    </row>
+    <row r="63" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E63" s="11"/>
+    </row>
+    <row r="64" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E64" s="11"/>
+    </row>
+    <row r="65" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E65" s="11"/>
+    </row>
+    <row r="66" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E66" s="11"/>
+    </row>
+    <row r="67" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E67" s="11"/>
+    </row>
+    <row r="68" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E68" s="11"/>
+    </row>
+    <row r="69" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E69" s="11"/>
+    </row>
+    <row r="70" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E70" s="11"/>
+    </row>
+    <row r="71" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E71" s="11"/>
+    </row>
+    <row r="72" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E72" s="11"/>
+    </row>
+    <row r="73" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E73" s="11"/>
+    </row>
+    <row r="74" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E74" s="11"/>
+    </row>
+    <row r="75" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E75" s="11"/>
+    </row>
+    <row r="76" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E76" s="11"/>
+    </row>
+    <row r="77" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E77" s="11"/>
+    </row>
+    <row r="78" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E78" s="11"/>
+    </row>
+    <row r="79" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E79" s="11"/>
+    </row>
+    <row r="80" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E80" s="11"/>
+    </row>
+    <row r="81" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E81" s="11"/>
+    </row>
+    <row r="82" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E82" s="11"/>
+    </row>
+    <row r="83" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E83" s="11"/>
+    </row>
+    <row r="84" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E84" s="11"/>
+    </row>
+    <row r="85" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E85" s="11"/>
+    </row>
+    <row r="86" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E86" s="11"/>
+    </row>
+    <row r="87" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E87" s="11"/>
+    </row>
+    <row r="88" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E88" s="11"/>
+    </row>
+    <row r="89" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E89" s="11"/>
+    </row>
+    <row r="90" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E90" s="11"/>
+    </row>
+    <row r="91" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E91" s="11"/>
+    </row>
+    <row r="92" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E92" s="11"/>
+    </row>
+    <row r="93" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E93" s="11"/>
+    </row>
+    <row r="94" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E94" s="11"/>
+    </row>
+    <row r="95" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E95" s="11"/>
+    </row>
+    <row r="96" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E96" s="11"/>
+    </row>
+    <row r="97" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E97" s="11"/>
+    </row>
+    <row r="98" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E98" s="11"/>
+    </row>
+    <row r="99" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E99" s="11"/>
+    </row>
+    <row r="100" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E100" s="11"/>
+    </row>
+    <row r="101" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E101" s="11"/>
+    </row>
+    <row r="102" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E102" s="11"/>
+    </row>
+    <row r="103" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E103" s="11"/>
+    </row>
+    <row r="104" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E104" s="11"/>
+    </row>
+    <row r="105" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E105" s="11"/>
+    </row>
+    <row r="106" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E106" s="11"/>
+    </row>
+    <row r="107" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E107" s="11"/>
+    </row>
+    <row r="108" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E108" s="11"/>
+    </row>
+    <row r="109" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E109" s="11"/>
+    </row>
+    <row r="110" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E110" s="11"/>
+    </row>
+    <row r="111" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E111" s="11"/>
+    </row>
+    <row r="112" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E112" s="11"/>
+    </row>
+    <row r="113" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E113" s="11"/>
+    </row>
+    <row r="114" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E114" s="11"/>
+    </row>
+    <row r="115" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E115" s="11"/>
+    </row>
+    <row r="116" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E116" s="11"/>
+    </row>
+    <row r="117" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E117" s="11"/>
+    </row>
+    <row r="118" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E118" s="11"/>
+    </row>
+    <row r="119" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E119" s="11"/>
+    </row>
+    <row r="120" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E120" s="11"/>
+    </row>
+    <row r="121" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E121" s="11"/>
+    </row>
+    <row r="122" spans="5:5" ht="19.5" customHeight="1">
+      <c r="E122" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -717,18 +883,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -846,14 +1012,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55355ED5-586E-4056-A608-186212A9F173}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDF51D17-4309-4E1C-99FA-3375289BD1D0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -864,6 +1022,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55355ED5-586E-4056-A608-186212A9F173}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>